<commit_message>
fix getty endpoints (#70)
</commit_message>
<xml_diff>
--- a/django/bartocfast/fixtures/sparqlendpoints.xlsx
+++ b/django/bartocfast/fixtures/sparqlendpoints.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\itsc-pg2.storage.p.unibas.ch\ub-home$\hinder0000\Documents\GitHub\bartocgraphql\django\bartocgraphql\fixtures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\itsc-pg2.storage.p.unibas.ch\ub-home$\hinder0000\Documents\GitHub\bartocfast\django\bartocfast\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -57,29 +57,6 @@
   </si>
   <si>
     <t>timeout</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT ?subject ?predicate ?object
-WHERE {
-  ?subject skos:definition ?object .
-  ?subject ?predicate ?object .
-  FILTER regex(?object, "!!!SEARCHWORD!!!", "i")
-}</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT ?subject ?predicate ?object
-WHERE {
-  ?subject rdfs:label ?object .
-  ?subject ?predicate ?object .
-  FILTER regex(?object, "!!!SEARCHWORD!!!" , "i")
-} 
-LIMIT 100</t>
-  </si>
-  <si>
-    <t>Return subjects whose skos:definition contains searchword.</t>
-  </si>
-  <si>
-    <t>Return subjects whose rdfs:label contains searchword; limited to 100.</t>
   </si>
   <si>
     <t>Return subjects whose rdfs:label bif:contains searchword; ordered by score and limited to 100.
@@ -155,14 +132,14 @@
     <t>context</t>
   </si>
   <si>
-    <t>special</t>
+    <t>virtuoso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,14 +163,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -212,21 +181,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -505,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A4" sqref="A4:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +488,7 @@
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -530,13 +496,13 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
@@ -550,7 +516,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -558,49 +524,20 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="F3">
-        <v>111</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="D4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>222</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="135" x14ac:dyDescent="0.25">
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -635,7 +572,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -657,7 +594,7 @@
     </row>
     <row r="3" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -666,10 +603,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -710,7 +647,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -732,7 +669,7 @@
     </row>
     <row r="3" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -741,10 +678,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -785,7 +722,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -807,7 +744,7 @@
     </row>
     <row r="3" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -816,10 +753,10 @@
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F3">
         <v>0</v>

</xml_diff>